<commit_message>
# Conclusions 19 - Learning rate 0.002 (twice the default 0.001) - Results - still too fast - accuracy worse: product .995, but not .999 - Time took - slightly better than default learning rate 0.001 ### Conclusions going forward: - Go back to much lower learning rates - go back to 0.001
</commit_message>
<xml_diff>
--- a/output/19_learn_rate_0.002/best.xlsx
+++ b/output/19_learn_rate_0.002/best.xlsx
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.002</v>
+        <v>0.0001</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F2" t="n">
         <v>200</v>
@@ -501,40 +501,40 @@
         <v>100</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001</v>
+        <v>0.002</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9679999947547913</v>
+        <v>0.9937000274658203</v>
       </c>
       <c r="N2" t="n">
-        <v>238.105</v>
+        <v>105.559</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0041</v>
+        <v>0.0095</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0041</v>
+        <v>0.0094</v>
       </c>
       <c r="Q2" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="R2" t="n">
-        <v>6.803</v>
+        <v>7.54</v>
       </c>
       <c r="S2" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9962999820709229</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9950000047683716</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9957000017166138</v>
       </c>
     </row>
     <row r="3">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.002</v>
+        <v>0.0001</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="n">
         <v>200</v>
@@ -570,40 +570,40 @@
         <v>100</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0001</v>
+        <v>0.002</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9993000030517578</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9679999947547913</v>
+        <v>0.9973999857902527</v>
       </c>
       <c r="N3" t="n">
-        <v>238.105</v>
+        <v>166.16</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0041</v>
+        <v>0.006</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0041</v>
+        <v>0.006</v>
       </c>
       <c r="Q3" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="R3" t="n">
-        <v>6.803</v>
+        <v>7.9124</v>
       </c>
       <c r="S3" t="n">
-        <v>0.98580002784729</v>
+        <v>0.998199999332428</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9947999715805054</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9980999827384949</v>
       </c>
     </row>
     <row r="4">
@@ -616,13 +616,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.002</v>
+        <v>0.0001</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F4" t="n">
         <v>200</v>
@@ -639,40 +639,40 @@
         <v>100</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0001</v>
+        <v>0.002</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9679999947547913</v>
+        <v>0.9937000274658203</v>
       </c>
       <c r="N4" t="n">
-        <v>238.105</v>
+        <v>105.559</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0041</v>
+        <v>0.0095</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0041</v>
+        <v>0.0094</v>
       </c>
       <c r="Q4" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="R4" t="n">
-        <v>6.803</v>
+        <v>7.54</v>
       </c>
       <c r="S4" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9962999820709229</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9950000047683716</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9957000017166138</v>
       </c>
     </row>
     <row r="5">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.002</v>
+        <v>0.0001</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F5" t="n">
         <v>200</v>
@@ -708,40 +708,40 @@
         <v>100</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0001</v>
+        <v>0.002</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9993000030517578</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9679999947547913</v>
+        <v>0.9973999857902527</v>
       </c>
       <c r="N5" t="n">
-        <v>238.105</v>
+        <v>166.16</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0041</v>
+        <v>0.006</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0041</v>
+        <v>0.006</v>
       </c>
       <c r="Q5" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="R5" t="n">
-        <v>6.803</v>
+        <v>7.9124</v>
       </c>
       <c r="S5" t="n">
-        <v>0.98580002784729</v>
+        <v>0.998199999332428</v>
       </c>
       <c r="T5" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9947999715805054</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9980999827384949</v>
       </c>
     </row>
     <row r="6">
@@ -754,13 +754,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.002</v>
+        <v>0.0001</v>
       </c>
       <c r="D6" t="n">
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F6" t="n">
         <v>200</v>
@@ -777,40 +777,40 @@
         <v>100</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0001</v>
+        <v>0.002</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9679999947547913</v>
+        <v>0.9937000274658203</v>
       </c>
       <c r="N6" t="n">
-        <v>238.105</v>
+        <v>105.559</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0041</v>
+        <v>0.0095</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0041</v>
+        <v>0.0094</v>
       </c>
       <c r="Q6" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="R6" t="n">
-        <v>6.803</v>
+        <v>7.54</v>
       </c>
       <c r="S6" t="n">
-        <v>0.98580002784729</v>
+        <v>0.9962999820709229</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9950000047683716</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9818999767303467</v>
+        <v>0.9957000017166138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>